<commit_message>
Added function to generate net infested acres field.
</commit_message>
<xml_diff>
--- a/CHIS_Formulation_Codes.xlsx
+++ b/CHIS_Formulation_Codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIS\Projects\CHIS Invasive GeoDB testing\WildLands_Grid_System_20200427\grid-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CD5ECA-7C46-4AA5-A904-1287CDDB43D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCA2A9E-711F-43D8-A4B4-938F7A14586A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59400" yWindow="870" windowWidth="29040" windowHeight="15840" xr2:uid="{F33F78D5-78A7-496C-8078-4ED368920487}"/>
+    <workbookView xWindow="35190" yWindow="2505" windowWidth="21600" windowHeight="11385" xr2:uid="{F33F78D5-78A7-496C-8078-4ED368920487}"/>
   </bookViews>
   <sheets>
     <sheet name="Weed_Point" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="99">
   <si>
     <t>Code</t>
   </si>
@@ -228,6 +228,9 @@
     <t xml:space="preserve">Glyphosate </t>
   </si>
   <si>
+    <t>Chlorsulphuron</t>
+  </si>
+  <si>
     <t>Telar XP</t>
   </si>
   <si>
@@ -291,6 +294,9 @@
     <t>72112-4</t>
   </si>
   <si>
+    <t>Glyphosate/Triclopyr (RoundupProConcentrate 2%/ Garlon4Ultra 2%); Agridex 1% No Wet</t>
+  </si>
+  <si>
     <t>RoundupProConcentrate</t>
   </si>
   <si>
@@ -327,20 +333,20 @@
     <t>Glyphosate/Imazapyr (ProkozGlyphosatePro4 2%/ Polaris 1%); Agridex 1% No Wet</t>
   </si>
   <si>
+    <t>Glyphosate/Triclopyr (Aquamaster 2%/ Garlon4Ultra 2%); Agridex 1% No Wet</t>
+  </si>
+  <si>
+    <t>Glyphosate (Roundup Pro 2%) No Wet</t>
+  </si>
+  <si>
     <t>Glyphosate (RoundupProConcentrate 2%) No Wet</t>
-  </si>
-  <si>
-    <t>Chlorsulfuron </t>
-  </si>
-  <si>
-    <t>ProkozGlyphosatePro4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,13 +363,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF2F4F4F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -395,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -404,7 +403,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -766,9 +770,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C40" sqref="C40"/>
+      <selection pane="topRight" activeCell="A43" sqref="A43:Q43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,10 +872,10 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N2" s="1">
         <v>0.01</v>
@@ -899,10 +903,10 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N3" s="1">
         <v>0.01</v>
@@ -911,15 +915,15 @@
       <c r="P3" s="3"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>95</v>
+      <c r="B4" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>53</v>
@@ -933,10 +937,10 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N4" s="1">
         <v>0.01</v>
@@ -945,15 +949,15 @@
       <c r="P4" s="3"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>95</v>
+      <c r="B5" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>53</v>
@@ -967,10 +971,10 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N5" s="1">
         <v>0.01</v>
@@ -984,10 +988,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>54</v>
@@ -1002,10 +1006,10 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N6" s="1">
         <v>0.01</v>
@@ -1019,10 +1023,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>54</v>
@@ -1037,10 +1041,10 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N7" s="1">
         <v>0.01</v>
@@ -1072,10 +1076,10 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N8" s="1">
         <v>0.01</v>
@@ -1107,10 +1111,10 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N9" s="1">
         <v>0.01</v>
@@ -1142,10 +1146,10 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N10" s="1">
         <v>0.33</v>
@@ -1177,10 +1181,10 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N11" s="1">
         <v>0.33</v>
@@ -1212,10 +1216,10 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N12" s="1">
         <v>0.5</v>
@@ -1253,10 +1257,10 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N13" s="1">
         <v>0.01</v>
@@ -1288,10 +1292,10 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N14" s="1">
         <v>0.01</v>
@@ -1323,10 +1327,10 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N15" s="1">
         <v>0.33</v>
@@ -1379,10 +1383,10 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N17" s="1">
         <v>0.01</v>
@@ -1414,10 +1418,10 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N18" s="1">
         <v>0.01</v>
@@ -1449,10 +1453,10 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N19" s="1">
         <v>0.5</v>
@@ -1492,10 +1496,10 @@
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N20" s="1">
         <v>0.01</v>
@@ -1527,10 +1531,10 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N21" s="1">
         <v>0.5</v>
@@ -1562,10 +1566,10 @@
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N22" s="1">
         <v>0.01</v>
@@ -1597,10 +1601,10 @@
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N23" s="1">
         <v>0.01</v>
@@ -1632,10 +1636,10 @@
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N24" s="1">
         <v>0.01</v>
@@ -1667,10 +1671,10 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N25" s="1">
         <v>0.5</v>
@@ -1681,7 +1685,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>44</v>
@@ -1700,20 +1704,20 @@
         <v>52</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J26" s="1">
         <v>0.02</v>
       </c>
       <c r="K26" s="1"/>
       <c r="L26" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N26" s="1">
         <v>0.01</v>
@@ -1724,7 +1728,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>49</v>
@@ -1753,10 +1757,10 @@
       </c>
       <c r="K27" s="1"/>
       <c r="L27" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N27" s="1">
         <v>0.01</v>
@@ -1767,16 +1771,16 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>60</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E28" s="1">
         <v>0.02</v>
@@ -1796,16 +1800,16 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>60</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E29" s="1">
         <v>0.02</v>
@@ -1825,10 +1829,10 @@
       </c>
       <c r="K29" s="1"/>
       <c r="L29" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N29" s="1">
         <v>0.01</v>
@@ -1839,7 +1843,7 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>44</v>
@@ -1868,10 +1872,10 @@
       </c>
       <c r="K30" s="1"/>
       <c r="L30" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N30" s="1">
         <v>0.01</v>
@@ -1882,7 +1886,7 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>44</v>
@@ -1911,10 +1915,10 @@
       </c>
       <c r="K31" s="1"/>
       <c r="L31" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N31" s="1">
         <v>0.01</v>
@@ -1925,16 +1929,16 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>60</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E32" s="1">
         <v>0.02</v>
@@ -1954,36 +1958,50 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>60</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E33" s="1">
         <v>0.02</v>
       </c>
       <c r="F33" s="1"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="1"/>
+      <c r="G33" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J33" s="1">
+        <v>0.02</v>
+      </c>
       <c r="K33" s="1"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="1"/>
+      <c r="L33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M33" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="N33" s="1">
+        <v>0.01</v>
+      </c>
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
       <c r="Q33" s="1"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>49</v>
@@ -2012,10 +2030,10 @@
       </c>
       <c r="K34" s="1"/>
       <c r="L34" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N34" s="1">
         <v>0.01</v>
@@ -2026,16 +2044,16 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E35" s="1">
         <v>0.03</v>
@@ -2055,16 +2073,16 @@
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E36" s="1">
         <v>0.02</v>
@@ -2084,10 +2102,10 @@
       </c>
       <c r="K36" s="1"/>
       <c r="L36" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N36" s="1">
         <v>0.01</v>
@@ -2098,7 +2116,7 @@
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>44</v>
@@ -2119,10 +2137,10 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N37" s="1">
         <v>0.01</v>
@@ -2133,16 +2151,16 @@
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E38" s="1">
         <v>0.02</v>
@@ -2162,16 +2180,16 @@
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E39" s="1">
         <v>0.02</v>
@@ -2191,10 +2209,10 @@
       </c>
       <c r="K39" s="1"/>
       <c r="L39" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N39" s="1">
         <v>0.01</v>
@@ -2205,16 +2223,16 @@
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E40" s="1">
         <v>0.02</v>
@@ -2234,10 +2252,10 @@
       </c>
       <c r="K40" s="1"/>
       <c r="L40" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M40" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N40" s="1">
         <v>0.01</v>
@@ -2247,18 +2265,38 @@
       <c r="Q40" s="1"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="1"/>
+      <c r="A41" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0.02</v>
+      </c>
       <c r="F41" s="1"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="1"/>
+      <c r="G41" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J41" s="1">
+        <v>0.02</v>
+      </c>
       <c r="K41" s="1"/>
-      <c r="L41" s="3"/>
+      <c r="L41" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="M41" s="3"/>
       <c r="N41" s="1"/>
       <c r="O41" s="3"/>
@@ -2266,11 +2304,21 @@
       <c r="Q41" s="1"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="1"/>
+      <c r="A42" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0.02</v>
+      </c>
       <c r="F42" s="1"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
@@ -2285,23 +2333,33 @@
       <c r="Q42" s="1"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="1"/>
-      <c r="O43" s="3"/>
-      <c r="P43" s="3"/>
-      <c r="Q43" s="1"/>
+      <c r="A43" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E43" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="F43" s="4"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="5"/>
+      <c r="P43" s="5"/>
+      <c r="Q43" s="4"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
@@ -3065,7 +3123,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>